<commit_message>
rebuild for web 1
</commit_message>
<xml_diff>
--- a/BATCH_QUESTION.xlsx
+++ b/BATCH_QUESTION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\exam-bank\frontend\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bokzg\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E923C200-EEE3-434A-BF5E-CCC4F19CA61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A48C22F-C4DA-47DB-AC0C-104D31A61032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E780121C-2525-404C-9D4A-6B3AD9A0A839}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E780121C-2525-404C-9D4A-6B3AD9A0A839}"/>
   </bookViews>
   <sheets>
     <sheet name="FORMAT" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>Classification</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>SA</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Terms</t>
   </si>
 </sst>
 </file>
@@ -338,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -363,9 +369,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -722,7 +725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446FE800-9452-4C2B-A21B-4868AD0CF6D1}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -744,36 +747,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="16"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -890,44 +893,44 @@
         <v>17</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -983,14 +986,14 @@
       <c r="E15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
       <c r="L15" s="8" t="s">
         <v>38</v>
       </c>
@@ -1015,12 +1018,12 @@
         <v>0</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
       <c r="L16" s="8">
         <v>3</v>
       </c>
@@ -1041,14 +1044,14 @@
       <c r="E17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
       <c r="L17" s="8" t="s">
         <v>42</v>
       </c>
@@ -1100,28 +1103,28 @@
       <c r="L19" s="2"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1144,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57513EB9-568B-43B7-9147-7A449078291A}">
   <dimension ref="A1:S320"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,33 +1162,34 @@
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="13" width="10.7109375" customWidth="1"/>
+    <col min="10" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1222,15 +1226,17 @@
         <v>34</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
+        <v>59</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="16"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>